<commit_message>
Update hs cost calculation
</commit_message>
<xml_diff>
--- a/Heat transition tipping pathways/_heating_system_data.xlsx
+++ b/Heat transition tipping pathways/_heating_system_data.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s124129\Documents\GitHub\Tipping-pathways\Heat transition neighborhood\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s124129\Documents\GitHub\Heat_transition_tipping_pathways\Heat transition tipping pathways\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{483EF4E8-8CD3-420B-92FA-4765A5F65FD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B595F6F0-1D1D-448D-9FE3-12084237151F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="1284" windowWidth="23256" windowHeight="12576" xr2:uid="{F2133ED2-96E7-4F18-A093-754F4E711694}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{F2133ED2-96E7-4F18-A093-754F4E711694}"/>
   </bookViews>
   <sheets>
     <sheet name="heating_system_data" sheetId="1" r:id="rId1"/>
+    <sheet name="energy_source_data" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="33">
   <si>
     <t>type</t>
   </si>
@@ -77,9 +78,6 @@
     <t>capex_eur_kW</t>
   </si>
   <si>
-    <t>opex_eur_kWh</t>
-  </si>
-  <si>
     <t>lifetime_years</t>
   </si>
   <si>
@@ -87,16 +85,68 @@
   </si>
   <si>
     <t>learning_rate_per_unit</t>
+  </si>
+  <si>
+    <t>energy_source_primary</t>
+  </si>
+  <si>
+    <t>energy_source_secondary</t>
+  </si>
+  <si>
+    <t>NATURAL_GAS</t>
+  </si>
+  <si>
+    <t>ELECTRICITY</t>
+  </si>
+  <si>
+    <t>NOT_APPLICABLE</t>
+  </si>
+  <si>
+    <t>HEAT</t>
+  </si>
+  <si>
+    <t>energy_source</t>
+  </si>
+  <si>
+    <t>costs_eur_per_kWh</t>
+  </si>
+  <si>
+    <t>cost_trend</t>
+  </si>
+  <si>
+    <t>source</t>
+  </si>
+  <si>
+    <t>https://ec.europa.eu/eurostat/databrowser/view/ten00117/default/table</t>
+  </si>
+  <si>
+    <t>https://ec.europa.eu/eurostat/databrowser/view/ten00118/default/table?lang=en&amp;category=t_nrg.t_nrg_indic</t>
+  </si>
+  <si>
+    <t>Niet meer dan anders principe</t>
+  </si>
+  <si>
+    <t>efficiency_primary_source</t>
+  </si>
+  <si>
+    <t>maintenance_costs_eur_k_wh</t>
+  </si>
+  <si>
+    <t>fraction_primary_energy_source</t>
+  </si>
+  <si>
+    <t>fraction_secondary_energy_source</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0%"/>
+    <numFmt numFmtId="165" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -110,6 +160,12 @@
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -133,10 +189,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -472,19 +533,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3AC4DA0D-C6DF-484D-B37A-107CF229F256}">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:N6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M16" sqref="M16"/>
+      <selection activeCell="N4" sqref="N4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="6" max="6" width="9.140625" style="1"/>
-    <col min="7" max="7" width="9.140625" style="2"/>
+    <col min="7" max="7" width="9.109375" style="1"/>
+    <col min="8" max="8" width="9.109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -494,132 +555,313 @@
       <c r="C1" t="s">
         <v>12</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1" t="s">
         <v>13</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="H1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="I1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K1" t="s">
+        <v>29</v>
+      </c>
+      <c r="L1" t="s">
+        <v>29</v>
+      </c>
+      <c r="M1" t="s">
+        <v>31</v>
+      </c>
+      <c r="N1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2" t="s">
         <v>7</v>
       </c>
-      <c r="C2">
-        <v>10000</v>
+      <c r="C2" s="3">
+        <v>1200</v>
       </c>
       <c r="D2">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="E2">
-        <v>15</v>
-      </c>
-      <c r="F2" s="1">
+        <v>12</v>
+      </c>
+      <c r="G2" s="1">
         <v>0.02</v>
       </c>
-      <c r="G2" s="2">
-        <v>1E-3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H2" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="I2" t="s">
+        <v>18</v>
+      </c>
+      <c r="J2" t="s">
+        <v>20</v>
+      </c>
+      <c r="K2" s="1">
+        <v>0.99</v>
+      </c>
+      <c r="L2" s="1">
+        <v>0</v>
+      </c>
+      <c r="M2">
+        <v>1</v>
+      </c>
+      <c r="N2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="B3" t="s">
         <v>8</v>
       </c>
-      <c r="C3">
-        <v>10000</v>
+      <c r="C3" s="3">
+        <v>1500</v>
       </c>
       <c r="D3">
-        <v>1100</v>
+        <v>0</v>
       </c>
       <c r="E3">
-        <v>15</v>
-      </c>
-      <c r="F3" s="1">
+        <v>20</v>
+      </c>
+      <c r="G3" s="1">
         <v>0.02</v>
       </c>
-      <c r="G3" s="2">
-        <v>1E-3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H3" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="I3" t="s">
+        <v>18</v>
+      </c>
+      <c r="J3" t="s">
+        <v>20</v>
+      </c>
+      <c r="K3" s="1">
+        <v>0.95</v>
+      </c>
+      <c r="L3" s="1">
+        <v>0</v>
+      </c>
+      <c r="M3">
+        <v>1</v>
+      </c>
+      <c r="N3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
       <c r="B4" t="s">
         <v>11</v>
       </c>
-      <c r="C4">
-        <v>9000</v>
+      <c r="C4" s="3">
+        <v>4500</v>
       </c>
       <c r="D4">
-        <v>600</v>
+        <v>0</v>
       </c>
       <c r="E4">
         <v>15</v>
       </c>
-      <c r="F4" s="1">
+      <c r="G4" s="1">
         <v>0.02</v>
       </c>
-      <c r="G4" s="2">
-        <v>1E-3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H4" s="2">
+        <v>0.15</v>
+      </c>
+      <c r="I4" t="s">
+        <v>19</v>
+      </c>
+      <c r="J4" t="s">
+        <v>18</v>
+      </c>
+      <c r="K4" s="1">
+        <v>3</v>
+      </c>
+      <c r="L4" s="1">
+        <v>0.99</v>
+      </c>
+      <c r="M4">
+        <v>0.8</v>
+      </c>
+      <c r="N4">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>4</v>
       </c>
       <c r="B5" t="s">
         <v>9</v>
       </c>
-      <c r="C5">
-        <v>8000</v>
+      <c r="C5" s="3">
+        <v>9000</v>
       </c>
       <c r="D5">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="E5">
         <v>15</v>
       </c>
-      <c r="F5" s="1">
+      <c r="G5" s="1">
         <v>0.02</v>
       </c>
-      <c r="G5" s="2">
-        <v>1E-3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H5" s="2">
+        <v>0.15</v>
+      </c>
+      <c r="I5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J5" t="s">
+        <v>20</v>
+      </c>
+      <c r="K5" s="1">
+        <v>3</v>
+      </c>
+      <c r="L5" s="1">
+        <v>0</v>
+      </c>
+      <c r="M5">
+        <v>1</v>
+      </c>
+      <c r="N5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>5</v>
       </c>
       <c r="B6" t="s">
         <v>10</v>
       </c>
-      <c r="C6">
-        <v>12000</v>
+      <c r="C6" s="3">
+        <v>5250.24</v>
       </c>
       <c r="D6">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="E6">
         <v>30</v>
       </c>
-      <c r="F6" s="1">
+      <c r="G6" s="1">
         <v>0.03</v>
       </c>
-      <c r="G6" s="2">
+      <c r="H6" s="2">
+        <v>0.08</v>
+      </c>
+      <c r="I6" t="s">
+        <v>21</v>
+      </c>
+      <c r="J6" t="s">
+        <v>20</v>
+      </c>
+      <c r="K6" s="1">
+        <v>0.8</v>
+      </c>
+      <c r="L6" s="1">
+        <v>0</v>
+      </c>
+      <c r="M6">
+        <v>1</v>
+      </c>
+      <c r="N6">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF8E5AC9-2AF6-4879-90A4-F2E8296BD951}">
+  <dimension ref="A1:D4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="4">
+        <f>45.1528*(3.6/1000)</f>
+        <v>0.16255007999999999</v>
+      </c>
+      <c r="C2" s="1">
         <v>0.01</v>
+      </c>
+      <c r="D2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3">
+        <v>0.26950000000000002</v>
+      </c>
+      <c r="C3" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="D3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" s="4">
+        <f>B2</f>
+        <v>0.16255007999999999</v>
+      </c>
+      <c r="C4" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="D4" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finished comparator and adoption
To do: get more heterogeneity in available heating methods and costs - could be based on hestia and TVW
</commit_message>
<xml_diff>
--- a/Heat transition tipping pathways/_heating_system_data.xlsx
+++ b/Heat transition tipping pathways/_heating_system_data.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s124129\Documents\GitHub\Heat_transition_tipping_pathways\Heat transition tipping pathways\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B595F6F0-1D1D-448D-9FE3-12084237151F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECA4C8D0-A5D4-437C-93C0-4982D871BA12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{F2133ED2-96E7-4F18-A093-754F4E711694}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{F2133ED2-96E7-4F18-A093-754F4E711694}"/>
   </bookViews>
   <sheets>
     <sheet name="heating_system_data" sheetId="1" r:id="rId1"/>
-    <sheet name="energy_source_data" sheetId="2" r:id="rId2"/>
+    <sheet name="insulation_data" sheetId="3" r:id="rId2"/>
+    <sheet name="energy_source_data" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="59">
   <si>
     <t>type</t>
   </si>
@@ -75,9 +76,6 @@
     <t>hybrid air-water heat pump with electricity or natural gas</t>
   </si>
   <si>
-    <t>capex_eur_kW</t>
-  </si>
-  <si>
     <t>lifetime_years</t>
   </si>
   <si>
@@ -129,13 +127,94 @@
     <t>efficiency_primary_source</t>
   </si>
   <si>
-    <t>maintenance_costs_eur_k_wh</t>
-  </si>
-  <si>
     <t>fraction_primary_energy_source</t>
   </si>
   <si>
     <t>fraction_secondary_energy_source</t>
+  </si>
+  <si>
+    <t>investment_costs_heat_supply_eur</t>
+  </si>
+  <si>
+    <t>investment_costs_heat_distribution_system_eur</t>
+  </si>
+  <si>
+    <t>maintenance_costs_eur_per_year</t>
+  </si>
+  <si>
+    <t>subsidy_eur</t>
+  </si>
+  <si>
+    <t>sustainability_score</t>
+  </si>
+  <si>
+    <t>Variable</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Value between 1-5 indicating perceived sustainability for consumers</t>
+  </si>
+  <si>
+    <t>ROOF</t>
+  </si>
+  <si>
+    <t>FACADE</t>
+  </si>
+  <si>
+    <t>CAVITY_WALL</t>
+  </si>
+  <si>
+    <t>FLOOR</t>
+  </si>
+  <si>
+    <t>rd_value_m2K_per_W</t>
+  </si>
+  <si>
+    <t>subsidy_eur_per_m2</t>
+  </si>
+  <si>
+    <t>ATTIC</t>
+  </si>
+  <si>
+    <t>max_surface_area_,2</t>
+  </si>
+  <si>
+    <t>* additional b onus for biobased materials is possible</t>
+  </si>
+  <si>
+    <t>U_W_per_m2K</t>
+  </si>
+  <si>
+    <t>GLASS_HR++</t>
+  </si>
+  <si>
+    <t>GLASS_TRIPLE</t>
+  </si>
+  <si>
+    <t>FRAMES_0.7</t>
+  </si>
+  <si>
+    <t>FRAMES_1.2</t>
+  </si>
+  <si>
+    <t>DOOR_1.5</t>
+  </si>
+  <si>
+    <t>DOOR_1.6</t>
+  </si>
+  <si>
+    <t>All data from ISDE rekentool 2024</t>
+  </si>
+  <si>
+    <t>efficiency_secondary_source</t>
+  </si>
+  <si>
+    <t>Min Value</t>
+  </si>
+  <si>
+    <t>Max Value</t>
   </si>
 </sst>
 </file>
@@ -146,7 +225,7 @@
     <numFmt numFmtId="164" formatCode="0.0%"/>
     <numFmt numFmtId="165" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -166,6 +245,12 @@
       <color rgb="FF000000"/>
       <name val="Consolas"/>
       <family val="3"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -533,19 +618,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3AC4DA0D-C6DF-484D-B37A-107CF229F256}">
-  <dimension ref="A1:N6"/>
+  <dimension ref="A1:P9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N4" sqref="N4"/>
+      <selection activeCell="P1" sqref="P1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="7" max="7" width="9.109375" style="1"/>
-    <col min="8" max="8" width="9.109375" style="2"/>
+    <col min="1" max="1" width="21.42578125" customWidth="1"/>
+    <col min="7" max="7" width="9.140625" style="1"/>
+    <col min="8" max="8" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -553,40 +639,49 @@
         <v>6</v>
       </c>
       <c r="C1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="F1" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="G1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J1" t="s">
+        <v>16</v>
+      </c>
+      <c r="K1" t="s">
+        <v>28</v>
+      </c>
+      <c r="L1" t="s">
+        <v>56</v>
+      </c>
+      <c r="M1" t="s">
+        <v>29</v>
+      </c>
+      <c r="N1" t="s">
         <v>30</v>
       </c>
-      <c r="E1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="I1" t="s">
-        <v>16</v>
-      </c>
-      <c r="J1" t="s">
-        <v>17</v>
-      </c>
-      <c r="K1" t="s">
-        <v>29</v>
-      </c>
-      <c r="L1" t="s">
-        <v>29</v>
-      </c>
-      <c r="M1" t="s">
-        <v>31</v>
-      </c>
-      <c r="N1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O1" t="s">
+        <v>34</v>
+      </c>
+      <c r="P1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -596,23 +691,26 @@
       <c r="C2" s="3">
         <v>1200</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="3">
         <v>0</v>
       </c>
       <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
         <v>12</v>
       </c>
       <c r="G2" s="1">
         <v>0.02</v>
       </c>
-      <c r="H2" s="2">
+      <c r="H2" s="1">
         <v>0.01</v>
       </c>
       <c r="I2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K2" s="1">
         <v>0.99</v>
@@ -626,8 +724,14 @@
       <c r="N2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O2">
+        <v>0</v>
+      </c>
+      <c r="P2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -637,23 +741,26 @@
       <c r="C3" s="3">
         <v>1500</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="3">
         <v>0</v>
       </c>
       <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
         <v>20</v>
       </c>
       <c r="G3" s="1">
         <v>0.02</v>
       </c>
-      <c r="H3" s="2">
+      <c r="H3" s="1">
         <v>0.01</v>
       </c>
       <c r="I3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K3" s="1">
         <v>0.95</v>
@@ -667,8 +774,14 @@
       <c r="N3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O3">
+        <v>0</v>
+      </c>
+      <c r="P3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -678,23 +791,26 @@
       <c r="C4" s="3">
         <v>4500</v>
       </c>
-      <c r="D4">
-        <v>0</v>
+      <c r="D4" s="3">
+        <v>5000</v>
       </c>
       <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
         <v>15</v>
       </c>
       <c r="G4" s="1">
         <v>0.02</v>
       </c>
-      <c r="H4" s="2">
+      <c r="H4" s="1">
         <v>0.15</v>
       </c>
       <c r="I4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K4" s="1">
         <v>3</v>
@@ -708,8 +824,14 @@
       <c r="N4">
         <v>0.2</v>
       </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O4">
+        <v>4000</v>
+      </c>
+      <c r="P4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -719,23 +841,26 @@
       <c r="C5" s="3">
         <v>9000</v>
       </c>
-      <c r="D5">
-        <v>0</v>
+      <c r="D5" s="3">
+        <v>5000</v>
       </c>
       <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
         <v>15</v>
       </c>
       <c r="G5" s="1">
         <v>0.02</v>
       </c>
-      <c r="H5" s="2">
+      <c r="H5" s="1">
         <v>0.15</v>
       </c>
       <c r="I5" t="s">
+        <v>18</v>
+      </c>
+      <c r="J5" t="s">
         <v>19</v>
-      </c>
-      <c r="J5" t="s">
-        <v>20</v>
       </c>
       <c r="K5" s="1">
         <v>3</v>
@@ -749,8 +874,14 @@
       <c r="N5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O5">
+        <v>4000</v>
+      </c>
+      <c r="P5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -760,23 +891,26 @@
       <c r="C6" s="3">
         <v>5250.24</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="3">
         <v>0</v>
       </c>
       <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
         <v>30</v>
       </c>
       <c r="G6" s="1">
         <v>0.03</v>
       </c>
-      <c r="H6" s="2">
+      <c r="H6" s="1">
         <v>0.08</v>
       </c>
       <c r="I6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K6" s="1">
         <v>0.8</v>
@@ -789,6 +923,40 @@
       </c>
       <c r="N6">
         <v>0</v>
+      </c>
+      <c r="O6">
+        <v>3775</v>
+      </c>
+      <c r="P6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>36</v>
+      </c>
+      <c r="B8" t="s">
+        <v>57</v>
+      </c>
+      <c r="C8" t="s">
+        <v>58</v>
+      </c>
+      <c r="D8" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9" s="3">
+        <v>5</v>
+      </c>
+      <c r="D9" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -797,6 +965,236 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13E48A5D-7E21-47C6-9DA6-E5FD725171EE}">
+  <dimension ref="A1:E21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L14" sqref="L14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2">
+        <v>3.5</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>30</v>
+      </c>
+      <c r="E2">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B3">
+        <v>3.5</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>8</v>
+      </c>
+      <c r="E3">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B4">
+        <v>3.5</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>38</v>
+      </c>
+      <c r="E4">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B5">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>8</v>
+      </c>
+      <c r="E5">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>42</v>
+      </c>
+      <c r="B6">
+        <v>3.5</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>6</v>
+      </c>
+      <c r="E6">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>49</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>1.2</v>
+      </c>
+      <c r="D7">
+        <v>46</v>
+      </c>
+      <c r="E7">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>50</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <v>0.7</v>
+      </c>
+      <c r="D8">
+        <v>131</v>
+      </c>
+      <c r="E8">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>53</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="C9">
+        <v>1.5</v>
+      </c>
+      <c r="D9">
+        <v>46</v>
+      </c>
+      <c r="E9">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>54</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10">
+        <v>131</v>
+      </c>
+      <c r="E10">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>52</v>
+      </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <v>1.2</v>
+      </c>
+      <c r="D11">
+        <v>20</v>
+      </c>
+      <c r="E11">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>51</v>
+      </c>
+      <c r="B12">
+        <v>0</v>
+      </c>
+      <c r="C12">
+        <v>0.7</v>
+      </c>
+      <c r="D12">
+        <v>90</v>
+      </c>
+      <c r="E12">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>47</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF8E5AC9-2AF6-4879-90A4-F2E8296BD951}">
   <dimension ref="A1:D4"/>
   <sheetViews>
@@ -804,25 +1202,25 @@
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" t="s">
         <v>22</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>23</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>24</v>
       </c>
-      <c r="D1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B2" s="4">
         <f>45.1528*(3.6/1000)</f>
@@ -832,12 +1230,12 @@
         <v>0.01</v>
       </c>
       <c r="D2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B3">
         <v>0.26950000000000002</v>
@@ -846,12 +1244,12 @@
         <v>0.01</v>
       </c>
       <c r="D3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B4" s="4">
         <f>B2</f>
@@ -861,7 +1259,7 @@
         <v>0.01</v>
       </c>
       <c r="D4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update data and loader
</commit_message>
<xml_diff>
--- a/Heat transition tipping pathways/_heating_system_data.xlsx
+++ b/Heat transition tipping pathways/_heating_system_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s124129\Documents\GitHub\Heat_transition_tipping_pathways\Heat transition tipping pathways\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECA4C8D0-A5D4-437C-93C0-4982D871BA12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4B06650-A779-443A-9FB6-75479E9371A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{F2133ED2-96E7-4F18-A093-754F4E711694}"/>
+    <workbookView xWindow="-23148" yWindow="1284" windowWidth="23256" windowHeight="12576" xr2:uid="{F2133ED2-96E7-4F18-A093-754F4E711694}"/>
   </bookViews>
   <sheets>
     <sheet name="heating_system_data" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="66">
   <si>
     <t>type</t>
   </si>
@@ -133,9 +133,6 @@
     <t>fraction_secondary_energy_source</t>
   </si>
   <si>
-    <t>investment_costs_heat_supply_eur</t>
-  </si>
-  <si>
     <t>investment_costs_heat_distribution_system_eur</t>
   </si>
   <si>
@@ -215,6 +212,30 @@
   </si>
   <si>
     <t>Max Value</t>
+  </si>
+  <si>
+    <t>investment_costs_eur_per_unit</t>
+  </si>
+  <si>
+    <t>investment_costs_eur_per_kw</t>
+  </si>
+  <si>
+    <t>kw_per_unit</t>
+  </si>
+  <si>
+    <t>costs_eur_per_kWh_eu</t>
+  </si>
+  <si>
+    <t>requiredDistributionSystem</t>
+  </si>
+  <si>
+    <t>LT, HT</t>
+  </si>
+  <si>
+    <t>HT</t>
+  </si>
+  <si>
+    <t>LT</t>
   </si>
 </sst>
 </file>
@@ -618,20 +639,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3AC4DA0D-C6DF-484D-B37A-107CF229F256}">
-  <dimension ref="A1:P9"/>
+  <dimension ref="A1:S9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P1" sqref="P1"/>
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21.42578125" customWidth="1"/>
-    <col min="7" max="7" width="9.140625" style="1"/>
-    <col min="8" max="8" width="9.140625" style="2"/>
+    <col min="10" max="10" width="9.140625" style="1"/>
+    <col min="11" max="11" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -639,49 +660,58 @@
         <v>6</v>
       </c>
       <c r="C1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E1" t="s">
+        <v>59</v>
+      </c>
+      <c r="F1" t="s">
+        <v>62</v>
+      </c>
+      <c r="G1" t="s">
         <v>31</v>
       </c>
-      <c r="D1" t="s">
+      <c r="H1" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="I1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="L1" t="s">
+        <v>15</v>
+      </c>
+      <c r="M1" t="s">
+        <v>16</v>
+      </c>
+      <c r="N1" t="s">
+        <v>28</v>
+      </c>
+      <c r="O1" t="s">
+        <v>55</v>
+      </c>
+      <c r="P1" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>30</v>
+      </c>
+      <c r="R1" t="s">
         <v>33</v>
       </c>
-      <c r="F1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="I1" t="s">
-        <v>15</v>
-      </c>
-      <c r="J1" t="s">
-        <v>16</v>
-      </c>
-      <c r="K1" t="s">
-        <v>28</v>
-      </c>
-      <c r="L1" t="s">
-        <v>56</v>
-      </c>
-      <c r="M1" t="s">
-        <v>29</v>
-      </c>
-      <c r="N1" t="s">
-        <v>30</v>
-      </c>
-      <c r="O1" t="s">
+      <c r="S1" t="s">
         <v>34</v>
       </c>
-      <c r="P1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -691,47 +721,52 @@
       <c r="C2" s="3">
         <v>1200</v>
       </c>
-      <c r="D2" s="3">
-        <v>0</v>
-      </c>
-      <c r="E2">
-        <v>0</v>
-      </c>
-      <c r="F2">
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="G2" s="3">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2">
         <v>12</v>
       </c>
-      <c r="G2" s="1">
+      <c r="J2" s="1">
         <v>0.02</v>
       </c>
-      <c r="H2" s="1">
+      <c r="K2" s="1">
         <v>0.01</v>
       </c>
-      <c r="I2" t="s">
+      <c r="L2" t="s">
         <v>17</v>
       </c>
-      <c r="J2" t="s">
+      <c r="M2" t="s">
         <v>19</v>
       </c>
-      <c r="K2" s="1">
+      <c r="N2" s="1">
         <v>0.99</v>
       </c>
-      <c r="L2" s="1">
-        <v>0</v>
-      </c>
-      <c r="M2">
-        <v>1</v>
-      </c>
-      <c r="N2">
-        <v>0</v>
-      </c>
-      <c r="O2">
+      <c r="O2" s="1">
         <v>0</v>
       </c>
       <c r="P2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q2">
+        <v>0</v>
+      </c>
+      <c r="R2">
+        <v>0</v>
+      </c>
+      <c r="S2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -741,47 +776,52 @@
       <c r="C3" s="3">
         <v>1500</v>
       </c>
-      <c r="D3" s="3">
-        <v>0</v>
-      </c>
-      <c r="E3">
-        <v>0</v>
-      </c>
-      <c r="F3">
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="G3" s="3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3">
         <v>20</v>
       </c>
-      <c r="G3" s="1">
+      <c r="J3" s="1">
         <v>0.02</v>
       </c>
-      <c r="H3" s="1">
+      <c r="K3" s="1">
         <v>0.01</v>
       </c>
-      <c r="I3" t="s">
+      <c r="L3" t="s">
         <v>17</v>
       </c>
-      <c r="J3" t="s">
+      <c r="M3" t="s">
         <v>19</v>
       </c>
-      <c r="K3" s="1">
+      <c r="N3" s="1">
         <v>0.95</v>
       </c>
-      <c r="L3" s="1">
-        <v>0</v>
-      </c>
-      <c r="M3">
-        <v>1</v>
-      </c>
-      <c r="N3">
-        <v>0</v>
-      </c>
-      <c r="O3">
+      <c r="O3" s="1">
         <v>0</v>
       </c>
       <c r="P3">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q3">
+        <v>0</v>
+      </c>
+      <c r="R3">
+        <v>0</v>
+      </c>
+      <c r="S3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -791,47 +831,52 @@
       <c r="C4" s="3">
         <v>4500</v>
       </c>
-      <c r="D4" s="3">
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="G4" s="3">
         <v>5000</v>
       </c>
-      <c r="E4">
-        <v>0</v>
-      </c>
-      <c r="F4">
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
         <v>15</v>
       </c>
-      <c r="G4" s="1">
+      <c r="J4" s="1">
         <v>0.02</v>
       </c>
-      <c r="H4" s="1">
+      <c r="K4" s="1">
         <v>0.15</v>
       </c>
-      <c r="I4" t="s">
+      <c r="L4" t="s">
         <v>18</v>
       </c>
-      <c r="J4" t="s">
+      <c r="M4" t="s">
         <v>17</v>
       </c>
-      <c r="K4" s="1">
+      <c r="N4" s="1">
         <v>3</v>
       </c>
-      <c r="L4" s="1">
+      <c r="O4" s="1">
         <v>0.99</v>
       </c>
-      <c r="M4">
+      <c r="P4">
         <v>0.8</v>
       </c>
-      <c r="N4">
+      <c r="Q4">
         <v>0.2</v>
       </c>
-      <c r="O4">
+      <c r="R4">
         <v>4000</v>
       </c>
-      <c r="P4">
+      <c r="S4">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -841,47 +886,52 @@
       <c r="C5" s="3">
         <v>9000</v>
       </c>
-      <c r="D5" s="3">
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="G5" s="3">
         <v>5000</v>
       </c>
-      <c r="E5">
-        <v>0</v>
-      </c>
-      <c r="F5">
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
         <v>15</v>
       </c>
-      <c r="G5" s="1">
+      <c r="J5" s="1">
         <v>0.02</v>
       </c>
-      <c r="H5" s="1">
+      <c r="K5" s="1">
         <v>0.15</v>
       </c>
-      <c r="I5" t="s">
+      <c r="L5" t="s">
         <v>18</v>
       </c>
-      <c r="J5" t="s">
+      <c r="M5" t="s">
         <v>19</v>
       </c>
-      <c r="K5" s="1">
+      <c r="N5" s="1">
         <v>3</v>
       </c>
-      <c r="L5" s="1">
-        <v>0</v>
-      </c>
-      <c r="M5">
+      <c r="O5" s="1">
+        <v>0</v>
+      </c>
+      <c r="P5">
         <v>1</v>
       </c>
-      <c r="N5">
-        <v>0</v>
-      </c>
-      <c r="O5">
+      <c r="Q5">
+        <v>0</v>
+      </c>
+      <c r="R5">
         <v>4000</v>
       </c>
-      <c r="P5">
+      <c r="S5">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -891,63 +941,68 @@
       <c r="C6" s="3">
         <v>5250.24</v>
       </c>
-      <c r="D6" s="3">
-        <v>0</v>
-      </c>
-      <c r="E6">
-        <v>0</v>
-      </c>
-      <c r="F6">
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="G6" s="3">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
         <v>30</v>
       </c>
-      <c r="G6" s="1">
+      <c r="J6" s="1">
         <v>0.03</v>
       </c>
-      <c r="H6" s="1">
+      <c r="K6" s="1">
         <v>0.08</v>
       </c>
-      <c r="I6" t="s">
+      <c r="L6" t="s">
         <v>20</v>
       </c>
-      <c r="J6" t="s">
+      <c r="M6" t="s">
         <v>19</v>
       </c>
-      <c r="K6" s="1">
+      <c r="N6" s="1">
         <v>0.8</v>
       </c>
-      <c r="L6" s="1">
-        <v>0</v>
-      </c>
-      <c r="M6">
+      <c r="O6" s="1">
+        <v>0</v>
+      </c>
+      <c r="P6">
         <v>1</v>
       </c>
-      <c r="N6">
-        <v>0</v>
-      </c>
-      <c r="O6">
+      <c r="Q6">
+        <v>0</v>
+      </c>
+      <c r="R6">
         <v>3775</v>
       </c>
-      <c r="P6">
+      <c r="S6">
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>35</v>
+      </c>
+      <c r="B8" t="s">
+        <v>56</v>
+      </c>
+      <c r="C8" t="s">
+        <v>57</v>
+      </c>
+      <c r="D8" t="s">
         <v>36</v>
       </c>
-      <c r="B8" t="s">
-        <v>57</v>
-      </c>
-      <c r="C8" t="s">
-        <v>58</v>
-      </c>
-      <c r="D8" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -956,8 +1011,10 @@
         <v>5</v>
       </c>
       <c r="D9" t="s">
-        <v>38</v>
-      </c>
+        <v>37</v>
+      </c>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -979,21 +1036,21 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D1" t="s">
         <v>43</v>
       </c>
-      <c r="C1" t="s">
-        <v>48</v>
-      </c>
-      <c r="D1" t="s">
-        <v>44</v>
-      </c>
       <c r="E1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B2">
         <v>3.5</v>
@@ -1010,7 +1067,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B3">
         <v>3.5</v>
@@ -1027,7 +1084,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B4">
         <v>3.5</v>
@@ -1044,7 +1101,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B5">
         <v>1.1000000000000001</v>
@@ -1061,7 +1118,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B6">
         <v>3.5</v>
@@ -1078,7 +1135,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -1095,7 +1152,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -1112,7 +1169,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B9">
         <v>0</v>
@@ -1129,7 +1186,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B10">
         <v>0</v>
@@ -1146,7 +1203,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B11">
         <v>0</v>
@@ -1163,7 +1220,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B12">
         <v>0</v>
@@ -1180,12 +1237,12 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -1196,15 +1253,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF8E5AC9-2AF6-4879-90A4-F2E8296BD951}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>21</v>
       </c>
@@ -1212,53 +1269,65 @@
         <v>22</v>
       </c>
       <c r="C1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D1" t="s">
         <v>23</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="4">
+      <c r="B2">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="C2" s="4">
         <f>45.1528*(3.6/1000)</f>
         <v>0.16255007999999999</v>
       </c>
-      <c r="C2" s="1">
+      <c r="D2" s="1">
         <v>0.01</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>18</v>
       </c>
       <c r="B3">
+        <v>0.32</v>
+      </c>
+      <c r="C3">
         <v>0.26950000000000002</v>
       </c>
-      <c r="C3" s="1">
+      <c r="D3" s="1">
         <v>0.01</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>20</v>
       </c>
-      <c r="B4" s="4">
-        <f>B2</f>
+      <c r="B4">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="C4" s="4">
+        <f>C2</f>
         <v>0.16255007999999999</v>
       </c>
-      <c r="C4" s="1">
+      <c r="D4" s="1">
         <v>0.01</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>27</v>
       </c>
     </row>

</xml_diff>